<commit_message>
image counter 1-12, do not break on skip number
</commit_message>
<xml_diff>
--- a/avito - csvv.xlsx
+++ b/avito - csvv.xlsx
@@ -234,9 +234,6 @@
     <t>https://i.ibb.co/s6ZcYJ2/1497281435-1.jpg, https://i.ibb.co/xzvX7gn/1497281435-2.jpg, https://i.ibb.co/SRCJbDr/1497281435-3.jpg</t>
   </si>
   <si>
-    <t>https://i.ibb.co/DRqzVDm/909190092-1.jpg, https://i.ibb.co/vB5Gfk1/909190092-2.jpg</t>
-  </si>
-  <si>
     <t>https://i.ibb.co/fD4Csfd/1242614238-1.jpg, https://i.ibb.co/VY1SCHm/1242614238-2.jpg, https://i.ibb.co/Qjf0FSF/1242614238-3.jpg, https://i.ibb.co/R22s7m2/1242614238-4.jpg, https://i.ibb.co/Q8wXKxD/1242614238-5.jpg</t>
   </si>
   <si>
@@ -256,6 +253,9 @@
   </si>
   <si>
     <t>https://i.ibb.co/spS12T3/1518506378-1.jpg, https://i.ibb.co/pvZ7f3n/1518506378-2.jpg</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/vB5Gfk1/909190092-2.jpg</t>
   </si>
 </sst>
 </file>
@@ -1256,7 +1256,7 @@
         <v>43580.638194444444</v>
       </c>
       <c r="J5" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="K5" t="s">
         <v>17</v>
@@ -1291,7 +1291,7 @@
         <v>43578.77847222222</v>
       </c>
       <c r="J6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K6" t="s">
         <v>17</v>
@@ -1326,7 +1326,7 @@
         <v>43575.502083333333</v>
       </c>
       <c r="J7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K7" t="s">
         <v>17</v>
@@ -1361,7 +1361,7 @@
         <v>43573.519444444442</v>
       </c>
       <c r="J8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K8" t="s">
         <v>17</v>
@@ -1396,7 +1396,7 @@
         <v>43577.720833333333</v>
       </c>
       <c r="J9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K9" t="s">
         <v>17</v>
@@ -1431,7 +1431,7 @@
         <v>43571.931250000001</v>
       </c>
       <c r="J10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K10" t="s">
         <v>17</v>
@@ -1466,7 +1466,7 @@
         <v>43567.582638888889</v>
       </c>
       <c r="J11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K11" t="s">
         <v>17</v>
@@ -1501,7 +1501,7 @@
         <v>43561.553472222222</v>
       </c>
       <c r="J12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K12" t="s">
         <v>17</v>

</xml_diff>